<commit_message>
upd fx_predict.xlsx by request
</commit_message>
<xml_diff>
--- a/sources/tables/fx_predict.xlsx
+++ b/sources/tables/fx_predict.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\sber\FinGigaChat\sources\tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\freek\GIT\FinGigaChat\sources\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6217312-DD40-45EE-B922-949D9C70DA84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85DCB52C-0FC8-446A-8FBE-9245D2DD323A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23700" yWindow="1710" windowWidth="25545" windowHeight="19185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Предсказание" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>EUR/USD</t>
   </si>
@@ -43,15 +43,9 @@
     <t>1к24</t>
   </si>
   <si>
-    <t xml:space="preserve"> USD/RUB</t>
-  </si>
-  <si>
     <t>CNY/RUB</t>
   </si>
   <si>
-    <t>3К23</t>
-  </si>
-  <si>
     <t>USD/CNY</t>
   </si>
   <si>
@@ -68,6 +62,15 @@
   </si>
   <si>
     <t>KZT/RUB*100</t>
+  </si>
+  <si>
+    <t>USD/RUB</t>
+  </si>
+  <si>
+    <t>2к24</t>
+  </si>
+  <si>
+    <t>4К23</t>
   </si>
 </sst>
 </file>
@@ -417,7 +420,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,33 +439,33 @@
         <v>5</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1">
-        <v>2023</v>
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1">
+        <v>98</v>
+      </c>
+      <c r="C2" s="1">
         <v>95</v>
-      </c>
-      <c r="C2" s="1">
-        <v>92</v>
       </c>
       <c r="D2" s="1">
         <v>90</v>
       </c>
       <c r="E2" s="1">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F2" s="1">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -470,19 +473,19 @@
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>1.0900000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="C3" s="1">
-        <v>1.0900000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="D3" s="1">
-        <v>1.0900000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="E3" s="1">
-        <v>1.1200000000000001</v>
+        <v>1.07</v>
       </c>
       <c r="F3" s="1">
-        <v>1.1299999999999999</v>
+        <v>1.0780000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -490,99 +493,99 @@
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>103.55</v>
+        <v>104.86</v>
       </c>
       <c r="C4" s="1">
-        <v>100.28</v>
+        <v>101.65</v>
       </c>
       <c r="D4" s="1">
-        <v>98.1</v>
+        <v>96.3</v>
       </c>
       <c r="E4" s="1">
-        <v>95.2</v>
+        <v>96.3</v>
       </c>
       <c r="F4" s="1">
-        <v>96.05</v>
+        <v>97.2</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="C5" s="1">
-        <v>7.2</v>
+        <v>7.3</v>
       </c>
       <c r="D5" s="1">
         <v>7.2</v>
       </c>
       <c r="E5" s="1">
+        <v>7.1</v>
+      </c>
+      <c r="F5" s="1">
         <v>7</v>
-      </c>
-      <c r="F5" s="1">
-        <v>6.8</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
-        <v>13.19</v>
+        <v>13.42</v>
       </c>
       <c r="C6" s="1">
-        <v>12.78</v>
+        <v>13.01</v>
       </c>
       <c r="D6" s="1">
         <v>12.5</v>
       </c>
       <c r="E6" s="1">
-        <v>12.14</v>
+        <v>12.68</v>
       </c>
       <c r="F6" s="1">
-        <v>12.5</v>
+        <v>12.86</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" s="1">
-        <v>82.8</v>
+        <v>83</v>
       </c>
       <c r="C7" s="1">
-        <v>82.2</v>
+        <v>83</v>
       </c>
       <c r="D7" s="1">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E7" s="1">
-        <v>80.34</v>
+        <v>83</v>
       </c>
       <c r="F7" s="1">
-        <v>80.2</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="1">
-        <v>1.1499999999999999</v>
+        <v>1.18</v>
       </c>
       <c r="C8" s="1">
-        <v>1.1200000000000001</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="D8" s="1">
-        <v>1.1000000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="E8" s="1">
-        <v>1.06</v>
+        <v>1.08</v>
       </c>
       <c r="F8" s="1">
-        <v>1.06</v>
+        <v>1.08</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -590,79 +593,79 @@
         <v>2</v>
       </c>
       <c r="B9" s="1">
-        <v>27</v>
+        <v>27.5</v>
       </c>
       <c r="C9" s="1">
+        <v>27.5</v>
+      </c>
+      <c r="D9" s="1">
         <v>28</v>
       </c>
-      <c r="D9" s="1">
+      <c r="E9" s="1">
         <v>29</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>30</v>
-      </c>
-      <c r="F9" s="1">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="1">
-        <v>3.52</v>
+        <v>3.56</v>
       </c>
       <c r="C10" s="1">
-        <v>3.29</v>
+        <v>3.45</v>
       </c>
       <c r="D10" s="1">
+        <v>3.21</v>
+      </c>
+      <c r="E10" s="1">
         <v>3.1</v>
       </c>
-      <c r="E10" s="1">
-        <v>2.83</v>
-      </c>
       <c r="F10" s="1">
-        <v>2.66</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="1">
-        <v>445</v>
+        <v>480</v>
       </c>
       <c r="C11" s="1">
-        <v>450</v>
+        <v>480</v>
       </c>
       <c r="D11" s="1">
-        <v>450</v>
+        <v>480</v>
       </c>
       <c r="E11" s="1">
-        <v>448.4</v>
+        <v>480</v>
       </c>
       <c r="F11" s="1">
-        <v>455.2</v>
+        <v>480</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="1">
-        <v>21.35</v>
+        <v>20.420000000000002</v>
       </c>
       <c r="C12" s="1">
-        <v>20.440000000000001</v>
+        <v>19.79</v>
       </c>
       <c r="D12" s="1">
-        <v>20</v>
+        <v>18.75</v>
       </c>
       <c r="E12" s="1">
-        <v>18.96</v>
+        <v>18.75</v>
       </c>
       <c r="F12" s="1">
-        <v>18.670000000000002</v>
+        <v>18.75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>